<commit_message>
Added group column to experimental file: grouping1 and grouping2
</commit_message>
<xml_diff>
--- a/src/report_manager/apps/templates/files/ClinicalData__Pxxxxxxx.xlsx
+++ b/src/report_manager/apps/templates/files/ClinicalData__Pxxxxxxx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plh450/Clinical_Proteomics/CKG/CKG/src/report_manager/apps/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\work\ClinicalKnowledgeGraph(CKG)\code\src\report_manager\apps\templates\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBE9E01-6D71-0646-8D6A-27CC1410B7D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB57CBB-93F1-416F-A954-852062722771}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="31140" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>subject external_id</t>
   </si>
@@ -77,12 +77,6 @@
   </si>
   <si>
     <t>timepoint units</t>
-  </si>
-  <si>
-    <t>grouping1</t>
-  </si>
-  <si>
-    <t>grouping2</t>
   </si>
   <si>
     <t>tissue</t>
@@ -511,75 +505,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AB1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="37" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="37" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="44" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="44" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -636,10 +628,10 @@
         <v>18</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>23</v>
@@ -659,14 +651,8 @@
       <c r="AH1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -678,7 +664,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -690,7 +676,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="10" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>

</xml_diff>